<commit_message>
added new distributed.xlsx results, filtered out frozen runs
</commit_message>
<xml_diff>
--- a/distributed.xlsx
+++ b/distributed.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,11 @@
           <t>CPU-time [s]</t>
         </is>
       </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Seed</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -460,7 +465,10 @@
         <v>9</v>
       </c>
       <c r="G2" t="n">
-        <v>0.067</v>
+        <v>0.113</v>
+      </c>
+      <c r="I2" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -471,19 +479,22 @@
         <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>360</v>
+        <v>332</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="F3" t="n">
         <v>9</v>
       </c>
       <c r="G3" t="n">
-        <v>0.074</v>
+        <v>0.076</v>
+      </c>
+      <c r="I3" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -494,19 +505,22 @@
         <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>414</v>
+        <v>373</v>
       </c>
       <c r="D4" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>0.85</v>
+        <v>0.25</v>
       </c>
       <c r="F4" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G4" t="n">
-        <v>0.124</v>
+        <v>0.162</v>
+      </c>
+      <c r="I4" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="5">
@@ -517,19 +531,22 @@
         <v>20</v>
       </c>
       <c r="C5" t="n">
-        <v>332</v>
+        <v>368</v>
       </c>
       <c r="D5" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E5" t="n">
-        <v>0.25</v>
+        <v>0.55</v>
       </c>
       <c r="F5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" t="n">
-        <v>0.053</v>
+        <v>0.144</v>
+      </c>
+      <c r="I5" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -540,19 +557,22 @@
         <v>20</v>
       </c>
       <c r="C6" t="n">
-        <v>298</v>
+        <v>329</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F6" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6" t="n">
-        <v>0.063</v>
+        <v>0.16</v>
+      </c>
+      <c r="I6" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="7">
@@ -563,19 +583,22 @@
         <v>20</v>
       </c>
       <c r="C7" t="n">
-        <v>334</v>
+        <v>357</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F7" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G7" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="I7" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="8">
@@ -586,19 +609,22 @@
         <v>20</v>
       </c>
       <c r="C8" t="n">
-        <v>385</v>
+        <v>316</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" t="n">
-        <v>0.133</v>
+        <v>0.096</v>
+      </c>
+      <c r="I8" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="9">
@@ -609,19 +635,22 @@
         <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="F9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" t="n">
-        <v>0.11</v>
+        <v>0.075</v>
+      </c>
+      <c r="I9" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="10">
@@ -632,7 +661,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>368</v>
+        <v>303</v>
       </c>
       <c r="D10" t="n">
         <v>4</v>
@@ -641,10 +670,13 @@
         <v>0.2</v>
       </c>
       <c r="F10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.155</v>
+      </c>
+      <c r="I10" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="11">
@@ -655,19 +687,22 @@
         <v>20</v>
       </c>
       <c r="C11" t="n">
-        <v>374</v>
+        <v>262</v>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="F11" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G11" t="n">
-        <v>30.082</v>
+        <v>0.077</v>
+      </c>
+      <c r="I11" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="12">
@@ -678,19 +713,22 @@
         <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E12" t="n">
-        <v>0.25</v>
+        <v>0.55</v>
       </c>
       <c r="F12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" t="n">
-        <v>30.062</v>
+        <v>0.141</v>
+      </c>
+      <c r="I12" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="13">
@@ -701,19 +739,22 @@
         <v>20</v>
       </c>
       <c r="C13" t="n">
-        <v>373</v>
+        <v>354</v>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" t="n">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="F13" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G13" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.125</v>
+      </c>
+      <c r="I13" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -727,16 +768,19 @@
         <v>324</v>
       </c>
       <c r="D14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F14" t="n">
         <v>10</v>
       </c>
       <c r="G14" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.113</v>
+      </c>
+      <c r="I14" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="15">
@@ -747,19 +791,22 @@
         <v>20</v>
       </c>
       <c r="C15" t="n">
-        <v>321</v>
+        <v>356</v>
       </c>
       <c r="D15" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E15" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="F15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" t="n">
-        <v>0.065</v>
+        <v>0.076</v>
+      </c>
+      <c r="I15" t="n">
+        <v>82</v>
       </c>
     </row>
     <row r="16">
@@ -770,19 +817,22 @@
         <v>20</v>
       </c>
       <c r="C16" t="n">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G16" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.125</v>
+      </c>
+      <c r="I16" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="17">
@@ -793,19 +843,22 @@
         <v>20</v>
       </c>
       <c r="C17" t="n">
-        <v>368</v>
+        <v>293</v>
       </c>
       <c r="D17" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E17" t="n">
-        <v>0.55</v>
+        <v>0.15</v>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.091</v>
+      </c>
+      <c r="I17" t="n">
+        <v>108</v>
       </c>
     </row>
     <row r="18">
@@ -816,19 +869,22 @@
         <v>20</v>
       </c>
       <c r="C18" t="n">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D18" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E18" t="n">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
       <c r="F18" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G18" t="n">
-        <v>0.106</v>
+        <v>0.133</v>
+      </c>
+      <c r="I18" t="n">
+        <v>118</v>
       </c>
     </row>
     <row r="19">
@@ -839,19 +895,22 @@
         <v>20</v>
       </c>
       <c r="C19" t="n">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.101</v>
+      </c>
+      <c r="I19" t="n">
+        <v>124</v>
       </c>
     </row>
     <row r="20">
@@ -862,19 +921,22 @@
         <v>20</v>
       </c>
       <c r="C20" t="n">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="F20" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G20" t="n">
-        <v>0.065</v>
+        <v>0.094</v>
+      </c>
+      <c r="I20" t="n">
+        <v>134</v>
       </c>
     </row>
     <row r="21">
@@ -888,16 +950,19 @@
         <v>329</v>
       </c>
       <c r="D21" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="F21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G21" t="n">
-        <v>0.093</v>
+        <v>0.076</v>
+      </c>
+      <c r="I21" t="n">
+        <v>145</v>
       </c>
     </row>
     <row r="22">
@@ -908,19 +973,22 @@
         <v>20</v>
       </c>
       <c r="C22" t="n">
-        <v>331</v>
+        <v>355</v>
       </c>
       <c r="D22" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="F22" t="n">
         <v>9</v>
       </c>
       <c r="G22" t="n">
-        <v>0.092</v>
+        <v>0.076</v>
+      </c>
+      <c r="I22" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="23">
@@ -931,19 +999,22 @@
         <v>20</v>
       </c>
       <c r="C23" t="n">
-        <v>357</v>
+        <v>310</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G23" t="n">
-        <v>0.05</v>
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="I23" t="n">
+        <v>152</v>
       </c>
     </row>
     <row r="24">
@@ -954,19 +1025,22 @@
         <v>20</v>
       </c>
       <c r="C24" t="n">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="D24" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E24" t="n">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="F24" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G24" t="n">
-        <v>0.073</v>
+        <v>0.107</v>
+      </c>
+      <c r="I24" t="n">
+        <v>154</v>
       </c>
     </row>
     <row r="25">
@@ -977,19 +1051,22 @@
         <v>20</v>
       </c>
       <c r="C25" t="n">
-        <v>316</v>
+        <v>349</v>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F25" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G25" t="n">
-        <v>0.053</v>
+        <v>0.138</v>
+      </c>
+      <c r="I25" t="n">
+        <v>157</v>
       </c>
     </row>
     <row r="26">
@@ -1000,19 +1077,22 @@
         <v>20</v>
       </c>
       <c r="C26" t="n">
-        <v>346</v>
+        <v>305</v>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="F26" t="n">
+        <v>7</v>
+      </c>
+      <c r="G26" t="n">
         <v>0.1</v>
       </c>
-      <c r="F26" t="n">
-        <v>8</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.059</v>
+      <c r="I26" t="n">
+        <v>166</v>
       </c>
     </row>
     <row r="27">
@@ -1023,7 +1103,7 @@
         <v>20</v>
       </c>
       <c r="C27" t="n">
-        <v>342</v>
+        <v>383</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
@@ -1032,10 +1112,13 @@
         <v>0.05</v>
       </c>
       <c r="F27" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G27" t="n">
-        <v>0.051</v>
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="I27" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="28">
@@ -1046,19 +1129,22 @@
         <v>20</v>
       </c>
       <c r="C28" t="n">
-        <v>314</v>
+        <v>335</v>
       </c>
       <c r="D28" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E28" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G28" t="n">
-        <v>30.068</v>
+        <v>0.066</v>
+      </c>
+      <c r="I28" t="n">
+        <v>183</v>
       </c>
     </row>
     <row r="29">
@@ -1069,19 +1155,22 @@
         <v>20</v>
       </c>
       <c r="C29" t="n">
-        <v>303</v>
+        <v>343</v>
       </c>
       <c r="D29" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="F29" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G29" t="n">
-        <v>0.077</v>
+        <v>0.099</v>
+      </c>
+      <c r="I29" t="n">
+        <v>184</v>
       </c>
     </row>
     <row r="30">
@@ -1092,19 +1181,22 @@
         <v>20</v>
       </c>
       <c r="C30" t="n">
-        <v>262</v>
+        <v>334</v>
       </c>
       <c r="D30" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E30" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F30" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G30" t="n">
-        <v>0.039</v>
+        <v>0.183</v>
+      </c>
+      <c r="I30" t="n">
+        <v>185</v>
       </c>
     </row>
     <row r="31">
@@ -1115,19 +1207,22 @@
         <v>20</v>
       </c>
       <c r="C31" t="n">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E31" t="n">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="F31" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G31" t="n">
-        <v>0.054</v>
+        <v>0.129</v>
+      </c>
+      <c r="I31" t="n">
+        <v>191</v>
       </c>
     </row>
     <row r="32">
@@ -1138,19 +1233,22 @@
         <v>20</v>
       </c>
       <c r="C32" t="n">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="D32" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E32" t="n">
-        <v>0.55</v>
+        <v>0.2</v>
       </c>
       <c r="F32" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G32" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.104</v>
+      </c>
+      <c r="I32" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="33">
@@ -1161,19 +1259,22 @@
         <v>20</v>
       </c>
       <c r="C33" t="n">
-        <v>354</v>
+        <v>312</v>
       </c>
       <c r="D33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E33" t="n">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="F33" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G33" t="n">
-        <v>0.077</v>
+        <v>0.076</v>
+      </c>
+      <c r="I33" t="n">
+        <v>210</v>
       </c>
     </row>
     <row r="34">
@@ -1184,19 +1285,22 @@
         <v>20</v>
       </c>
       <c r="C34" t="n">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F34" t="n">
         <v>8</v>
       </c>
       <c r="G34" t="n">
         <v>0.07099999999999999</v>
+      </c>
+      <c r="I34" t="n">
+        <v>220</v>
       </c>
     </row>
     <row r="35">
@@ -1207,19 +1311,22 @@
         <v>20</v>
       </c>
       <c r="C35" t="n">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="D35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E35" t="n">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="F35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G35" t="n">
-        <v>0.066</v>
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="I35" t="n">
+        <v>230</v>
       </c>
     </row>
     <row r="36">
@@ -1230,19 +1337,22 @@
         <v>20</v>
       </c>
       <c r="C36" t="n">
-        <v>376</v>
+        <v>337</v>
       </c>
       <c r="D36" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E36" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="F36" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G36" t="n">
-        <v>0.108</v>
+        <v>0.123</v>
+      </c>
+      <c r="I36" t="n">
+        <v>236</v>
       </c>
     </row>
     <row r="37">
@@ -1253,19 +1363,22 @@
         <v>20</v>
       </c>
       <c r="C37" t="n">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="D37" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E37" t="n">
-        <v>0.75</v>
+        <v>0.05</v>
       </c>
       <c r="F37" t="n">
         <v>8</v>
       </c>
       <c r="G37" t="n">
-        <v>30.079</v>
+        <v>0.168</v>
+      </c>
+      <c r="I37" t="n">
+        <v>237</v>
       </c>
     </row>
     <row r="38">
@@ -1276,19 +1389,22 @@
         <v>20</v>
       </c>
       <c r="C38" t="n">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="D38" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E38" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G38" t="n">
-        <v>0.08400000000000001</v>
+        <v>0.192</v>
+      </c>
+      <c r="I38" t="n">
+        <v>243</v>
       </c>
     </row>
     <row r="39">
@@ -1299,19 +1415,22 @@
         <v>20</v>
       </c>
       <c r="C39" t="n">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E39" t="n">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="F39" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G39" t="n">
-        <v>0.068</v>
+        <v>0.14</v>
+      </c>
+      <c r="I39" t="n">
+        <v>247</v>
       </c>
     </row>
     <row r="40">
@@ -1322,19 +1441,22 @@
         <v>20</v>
       </c>
       <c r="C40" t="n">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F40" t="n">
         <v>8</v>
       </c>
       <c r="G40" t="n">
-        <v>0.068</v>
+        <v>0.107</v>
+      </c>
+      <c r="I40" t="n">
+        <v>256</v>
       </c>
     </row>
     <row r="41">
@@ -1345,19 +1467,22 @@
         <v>20</v>
       </c>
       <c r="C41" t="n">
-        <v>358</v>
+        <v>373</v>
       </c>
       <c r="D41" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E41" t="n">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="F41" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G41" t="n">
-        <v>0.121</v>
+        <v>0.075</v>
+      </c>
+      <c r="I41" t="n">
+        <v>266</v>
       </c>
     </row>
     <row r="42">
@@ -1368,19 +1493,22 @@
         <v>20</v>
       </c>
       <c r="C42" t="n">
-        <v>324</v>
+        <v>358</v>
       </c>
       <c r="D42" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E42" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F42" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G42" t="n">
-        <v>0.059</v>
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="I42" t="n">
+        <v>275</v>
       </c>
     </row>
     <row r="43">
@@ -1391,19 +1519,22 @@
         <v>20</v>
       </c>
       <c r="C43" t="n">
-        <v>329</v>
+        <v>354</v>
       </c>
       <c r="D43" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E43" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F43" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G43" t="n">
-        <v>0.051</v>
+        <v>0.106</v>
+      </c>
+      <c r="I43" t="n">
+        <v>282</v>
       </c>
     </row>
     <row r="44">
@@ -1414,7 +1545,7 @@
         <v>20</v>
       </c>
       <c r="C44" t="n">
-        <v>368</v>
+        <v>341</v>
       </c>
       <c r="D44" t="n">
         <v>2</v>
@@ -1423,10 +1554,13 @@
         <v>0.1</v>
       </c>
       <c r="F44" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G44" t="n">
-        <v>0.077</v>
+        <v>0.091</v>
+      </c>
+      <c r="I44" t="n">
+        <v>284</v>
       </c>
     </row>
     <row r="45">
@@ -1440,16 +1574,19 @@
         <v>352</v>
       </c>
       <c r="D45" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E45" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G45" t="n">
-        <v>30.074</v>
+        <v>0.123</v>
+      </c>
+      <c r="I45" t="n">
+        <v>292</v>
       </c>
     </row>
     <row r="46">
@@ -1460,19 +1597,22 @@
         <v>20</v>
       </c>
       <c r="C46" t="n">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="D46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E46" t="n">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="F46" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G46" t="n">
-        <v>0.116</v>
+        <v>0.089</v>
+      </c>
+      <c r="I46" t="n">
+        <v>296</v>
       </c>
     </row>
     <row r="47">
@@ -1483,19 +1623,22 @@
         <v>20</v>
       </c>
       <c r="C47" t="n">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="D47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F47" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G47" t="n">
-        <v>30.057</v>
+        <v>0.073</v>
+      </c>
+      <c r="I47" t="n">
+        <v>297</v>
       </c>
     </row>
     <row r="48">
@@ -1506,19 +1649,22 @@
         <v>20</v>
       </c>
       <c r="C48" t="n">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="D48" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
         <v>9</v>
       </c>
       <c r="G48" t="n">
-        <v>30.072</v>
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="I48" t="n">
+        <v>302</v>
       </c>
     </row>
     <row r="49">
@@ -1529,19 +1675,22 @@
         <v>20</v>
       </c>
       <c r="C49" t="n">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="D49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E49" t="n">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="F49" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G49" t="n">
-        <v>0.044</v>
+        <v>0.063</v>
+      </c>
+      <c r="I49" t="n">
+        <v>311</v>
       </c>
     </row>
     <row r="50">
@@ -1552,19 +1701,22 @@
         <v>20</v>
       </c>
       <c r="C50" t="n">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="D50" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
-        <v>0.35</v>
+        <v>0.05</v>
       </c>
       <c r="F50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G50" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.101</v>
+      </c>
+      <c r="I50" t="n">
+        <v>318</v>
       </c>
     </row>
     <row r="51">
@@ -1575,19 +1727,22 @@
         <v>20</v>
       </c>
       <c r="C51" t="n">
-        <v>356</v>
+        <v>386</v>
       </c>
       <c r="D51" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E51" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F51" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G51" t="n">
-        <v>0.049</v>
+        <v>0.102</v>
+      </c>
+      <c r="I51" t="n">
+        <v>326</v>
       </c>
     </row>
     <row r="52">
@@ -1598,19 +1753,22 @@
         <v>20</v>
       </c>
       <c r="C52" t="n">
-        <v>327</v>
+        <v>357</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F52" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G52" t="n">
-        <v>0.075</v>
+        <v>0.09</v>
+      </c>
+      <c r="I52" t="n">
+        <v>333</v>
       </c>
     </row>
     <row r="53">
@@ -1621,19 +1779,22 @@
         <v>20</v>
       </c>
       <c r="C53" t="n">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="D53" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E53" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="F53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G53" t="n">
-        <v>0.092</v>
+        <v>0.111</v>
+      </c>
+      <c r="I53" t="n">
+        <v>334</v>
       </c>
     </row>
     <row r="54">
@@ -1644,19 +1805,22 @@
         <v>20</v>
       </c>
       <c r="C54" t="n">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D54" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E54" t="n">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="F54" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G54" t="n">
-        <v>0.074</v>
+        <v>0.1</v>
+      </c>
+      <c r="I54" t="n">
+        <v>337</v>
       </c>
     </row>
     <row r="55">
@@ -1667,19 +1831,22 @@
         <v>20</v>
       </c>
       <c r="C55" t="n">
-        <v>345</v>
+        <v>306</v>
       </c>
       <c r="D55" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E55" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F55" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G55" t="n">
-        <v>0.08</v>
+        <v>0.082</v>
+      </c>
+      <c r="I55" t="n">
+        <v>340</v>
       </c>
     </row>
     <row r="56">
@@ -1690,19 +1857,22 @@
         <v>20</v>
       </c>
       <c r="C56" t="n">
-        <v>321</v>
+        <v>368</v>
       </c>
       <c r="D56" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E56" t="n">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="F56" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G56" t="n">
-        <v>0.051</v>
+        <v>0.119</v>
+      </c>
+      <c r="I56" t="n">
+        <v>349</v>
       </c>
     </row>
     <row r="57">
@@ -1713,19 +1883,22 @@
         <v>20</v>
       </c>
       <c r="C57" t="n">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="D57" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E57" t="n">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="F57" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G57" t="n">
-        <v>0.058</v>
+        <v>0.116</v>
+      </c>
+      <c r="I57" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="58">
@@ -1736,19 +1909,22 @@
         <v>20</v>
       </c>
       <c r="C58" t="n">
-        <v>336</v>
+        <v>358</v>
       </c>
       <c r="D58" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E58" t="n">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F58" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G58" t="n">
-        <v>0.064</v>
+        <v>0.126</v>
+      </c>
+      <c r="I58" t="n">
+        <v>354</v>
       </c>
     </row>
     <row r="59">
@@ -1759,19 +1935,22 @@
         <v>20</v>
       </c>
       <c r="C59" t="n">
-        <v>333</v>
+        <v>372</v>
       </c>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E59" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F59" t="n">
         <v>8</v>
       </c>
       <c r="G59" t="n">
-        <v>0.057</v>
+        <v>0.09</v>
+      </c>
+      <c r="I59" t="n">
+        <v>363</v>
       </c>
     </row>
     <row r="60">
@@ -1782,7 +1961,7 @@
         <v>20</v>
       </c>
       <c r="C60" t="n">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D60" t="n">
         <v>7</v>
@@ -1791,10 +1970,13 @@
         <v>0.35</v>
       </c>
       <c r="F60" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G60" t="n">
-        <v>0.12</v>
+        <v>0.167</v>
+      </c>
+      <c r="I60" t="n">
+        <v>373</v>
       </c>
     </row>
     <row r="61">
@@ -1805,19 +1987,22 @@
         <v>20</v>
       </c>
       <c r="C61" t="n">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="D61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E61" t="n">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F61" t="n">
         <v>9</v>
       </c>
       <c r="G61" t="n">
-        <v>0.051</v>
+        <v>0.079</v>
+      </c>
+      <c r="I61" t="n">
+        <v>391</v>
       </c>
     </row>
     <row r="62">
@@ -1828,19 +2013,22 @@
         <v>20</v>
       </c>
       <c r="C62" t="n">
-        <v>361</v>
+        <v>340</v>
       </c>
       <c r="D62" t="n">
+        <v>2</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F62" t="n">
         <v>9</v>
       </c>
-      <c r="E62" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="F62" t="n">
-        <v>11</v>
-      </c>
       <c r="G62" t="n">
-        <v>0.075</v>
+        <v>0.076</v>
+      </c>
+      <c r="I62" t="n">
+        <v>396</v>
       </c>
     </row>
     <row r="63">
@@ -1851,19 +2039,22 @@
         <v>20</v>
       </c>
       <c r="C63" t="n">
-        <v>332</v>
+        <v>355</v>
       </c>
       <c r="D63" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E63" t="n">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="F63" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G63" t="n">
-        <v>30.088</v>
+        <v>0.08</v>
+      </c>
+      <c r="I63" t="n">
+        <v>400</v>
       </c>
     </row>
     <row r="64">
@@ -1874,19 +2065,22 @@
         <v>20</v>
       </c>
       <c r="C64" t="n">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="D64" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E64" t="n">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="F64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G64" t="n">
-        <v>0.074</v>
+        <v>0.123</v>
+      </c>
+      <c r="I64" t="n">
+        <v>405</v>
       </c>
     </row>
     <row r="65">
@@ -1897,19 +2091,22 @@
         <v>20</v>
       </c>
       <c r="C65" t="n">
-        <v>367</v>
+        <v>383</v>
       </c>
       <c r="D65" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E65" t="n">
-        <v>0.45</v>
+        <v>0.1</v>
       </c>
       <c r="F65" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G65" t="n">
-        <v>0.109</v>
+        <v>0.128</v>
+      </c>
+      <c r="I65" t="n">
+        <v>417</v>
       </c>
     </row>
     <row r="66">
@@ -1920,19 +2117,22 @@
         <v>20</v>
       </c>
       <c r="C66" t="n">
-        <v>336</v>
+        <v>351</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F66" t="n">
         <v>8</v>
       </c>
       <c r="G66" t="n">
-        <v>0.054</v>
+        <v>0.11</v>
+      </c>
+      <c r="I66" t="n">
+        <v>431</v>
       </c>
     </row>
     <row r="67">
@@ -1943,19 +2143,22 @@
         <v>20</v>
       </c>
       <c r="C67" t="n">
-        <v>317</v>
+        <v>364</v>
       </c>
       <c r="D67" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G67" t="n">
-        <v>0.049</v>
+        <v>0.153</v>
+      </c>
+      <c r="I67" t="n">
+        <v>439</v>
       </c>
     </row>
     <row r="68">
@@ -1966,19 +2169,22 @@
         <v>20</v>
       </c>
       <c r="C68" t="n">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F68" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G68" t="n">
-        <v>0.045</v>
+        <v>0.107</v>
+      </c>
+      <c r="I68" t="n">
+        <v>451</v>
       </c>
     </row>
     <row r="69">
@@ -1989,7 +2195,7 @@
         <v>20</v>
       </c>
       <c r="C69" t="n">
-        <v>318</v>
+        <v>334</v>
       </c>
       <c r="D69" t="n">
         <v>2</v>
@@ -1998,10 +2204,13 @@
         <v>0.1</v>
       </c>
       <c r="F69" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G69" t="n">
-        <v>20.065</v>
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="I69" t="n">
+        <v>453</v>
       </c>
     </row>
     <row r="70">
@@ -2012,19 +2221,22 @@
         <v>20</v>
       </c>
       <c r="C70" t="n">
-        <v>319</v>
+        <v>352</v>
       </c>
       <c r="D70" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E70" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G70" t="n">
-        <v>0.062</v>
+        <v>0.099</v>
+      </c>
+      <c r="I70" t="n">
+        <v>464</v>
       </c>
     </row>
     <row r="71">
@@ -2035,19 +2247,22 @@
         <v>20</v>
       </c>
       <c r="C71" t="n">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="D71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E71" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F71" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G71" t="n">
-        <v>0.052</v>
+        <v>0.132</v>
+      </c>
+      <c r="I71" t="n">
+        <v>466</v>
       </c>
     </row>
     <row r="72">
@@ -2058,19 +2273,22 @@
         <v>20</v>
       </c>
       <c r="C72" t="n">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="D72" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E72" t="n">
-        <v>0.45</v>
+        <v>0.05</v>
       </c>
       <c r="F72" t="n">
         <v>9</v>
       </c>
       <c r="G72" t="n">
-        <v>0.103</v>
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="I72" t="n">
+        <v>468</v>
       </c>
     </row>
     <row r="73">
@@ -2081,19 +2299,22 @@
         <v>20</v>
       </c>
       <c r="C73" t="n">
-        <v>333</v>
+        <v>357</v>
       </c>
       <c r="D73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E73" t="n">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="F73" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G73" t="n">
-        <v>0.104</v>
+        <v>0.102</v>
+      </c>
+      <c r="I73" t="n">
+        <v>490</v>
       </c>
     </row>
     <row r="74">
@@ -2104,7 +2325,7 @@
         <v>20</v>
       </c>
       <c r="C74" t="n">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="D74" t="n">
         <v>2</v>
@@ -2113,10 +2334,13 @@
         <v>0.1</v>
       </c>
       <c r="F74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G74" t="n">
-        <v>0.08400000000000001</v>
+        <v>0.095</v>
+      </c>
+      <c r="I74" t="n">
+        <v>492</v>
       </c>
     </row>
     <row r="75">
@@ -2127,19 +2351,22 @@
         <v>20</v>
       </c>
       <c r="C75" t="n">
-        <v>329</v>
+        <v>371</v>
       </c>
       <c r="D75" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E75" t="n">
-        <v>0.15</v>
+        <v>0.45</v>
       </c>
       <c r="F75" t="n">
         <v>10</v>
       </c>
       <c r="G75" t="n">
-        <v>0.049</v>
+        <v>0.172</v>
+      </c>
+      <c r="I75" t="n">
+        <v>510</v>
       </c>
     </row>
     <row r="76">
@@ -2150,19 +2377,22 @@
         <v>20</v>
       </c>
       <c r="C76" t="n">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="F76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G76" t="n">
-        <v>0.055</v>
+        <v>0.134</v>
+      </c>
+      <c r="I76" t="n">
+        <v>516</v>
       </c>
     </row>
     <row r="77">
@@ -2173,19 +2403,22 @@
         <v>20</v>
       </c>
       <c r="C77" t="n">
-        <v>352</v>
+        <v>369</v>
       </c>
       <c r="D77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E77" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F77" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G77" t="n">
-        <v>0.059</v>
+        <v>0.068</v>
+      </c>
+      <c r="I77" t="n">
+        <v>519</v>
       </c>
     </row>
     <row r="78">
@@ -2196,19 +2429,22 @@
         <v>20</v>
       </c>
       <c r="C78" t="n">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="D78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G78" t="n">
-        <v>0.049</v>
+        <v>0.08599999999999999</v>
+      </c>
+      <c r="I78" t="n">
+        <v>523</v>
       </c>
     </row>
     <row r="79">
@@ -2219,19 +2455,22 @@
         <v>20</v>
       </c>
       <c r="C79" t="n">
-        <v>344</v>
+        <v>360</v>
       </c>
       <c r="D79" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E79" t="n">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="F79" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G79" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.2</v>
+      </c>
+      <c r="I79" t="n">
+        <v>531</v>
       </c>
     </row>
     <row r="80">
@@ -2242,19 +2481,22 @@
         <v>20</v>
       </c>
       <c r="C80" t="n">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D80" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E80" t="n">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="F80" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G80" t="n">
-        <v>0.103</v>
+        <v>0.144</v>
+      </c>
+      <c r="I80" t="n">
+        <v>542</v>
       </c>
     </row>
     <row r="81">
@@ -2265,19 +2507,22 @@
         <v>20</v>
       </c>
       <c r="C81" t="n">
-        <v>354</v>
+        <v>320</v>
       </c>
       <c r="D81" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E81" t="n">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="F81" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G81" t="n">
-        <v>0.081</v>
+        <v>0.117</v>
+      </c>
+      <c r="I81" t="n">
+        <v>552</v>
       </c>
     </row>
     <row r="82">
@@ -2288,19 +2533,22 @@
         <v>20</v>
       </c>
       <c r="C82" t="n">
-        <v>329</v>
+        <v>352</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E82" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F82" t="n">
         <v>9</v>
       </c>
       <c r="G82" t="n">
-        <v>0.054</v>
+        <v>0.109</v>
+      </c>
+      <c r="I82" t="n">
+        <v>581</v>
       </c>
     </row>
     <row r="83">
@@ -2311,19 +2559,22 @@
         <v>20</v>
       </c>
       <c r="C83" t="n">
-        <v>344</v>
+        <v>396</v>
       </c>
       <c r="D83" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E83" t="n">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="F83" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G83" t="n">
-        <v>0.083</v>
+        <v>0.126</v>
+      </c>
+      <c r="I83" t="n">
+        <v>583</v>
       </c>
     </row>
     <row r="84">
@@ -2334,19 +2585,22 @@
         <v>20</v>
       </c>
       <c r="C84" t="n">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="D84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E84" t="n">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="F84" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G84" t="n">
-        <v>0.106</v>
+        <v>0.097</v>
+      </c>
+      <c r="I84" t="n">
+        <v>592</v>
       </c>
     </row>
     <row r="85">
@@ -2357,19 +2611,22 @@
         <v>20</v>
       </c>
       <c r="C85" t="n">
-        <v>355</v>
+        <v>280</v>
       </c>
       <c r="D85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G85" t="n">
-        <v>0.041</v>
+        <v>0.089</v>
+      </c>
+      <c r="I85" t="n">
+        <v>594</v>
       </c>
     </row>
     <row r="86">
@@ -2380,19 +2637,22 @@
         <v>20</v>
       </c>
       <c r="C86" t="n">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="D86" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E86" t="n">
-        <v>0.05</v>
+        <v>0.35</v>
       </c>
       <c r="F86" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G86" t="n">
-        <v>0.067</v>
+        <v>0.08599999999999999</v>
+      </c>
+      <c r="I86" t="n">
+        <v>595</v>
       </c>
     </row>
     <row r="87">
@@ -2403,7 +2663,7 @@
         <v>20</v>
       </c>
       <c r="C87" t="n">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
@@ -2412,10 +2672,13 @@
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G87" t="n">
-        <v>0.052</v>
+        <v>0.061</v>
+      </c>
+      <c r="I87" t="n">
+        <v>607</v>
       </c>
     </row>
     <row r="88">
@@ -2426,19 +2689,22 @@
         <v>20</v>
       </c>
       <c r="C88" t="n">
-        <v>318</v>
+        <v>361</v>
       </c>
       <c r="D88" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E88" t="n">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="F88" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G88" t="n">
-        <v>0.057</v>
+        <v>0.098</v>
+      </c>
+      <c r="I88" t="n">
+        <v>609</v>
       </c>
     </row>
     <row r="89">
@@ -2449,19 +2715,22 @@
         <v>20</v>
       </c>
       <c r="C89" t="n">
-        <v>390</v>
+        <v>341</v>
       </c>
       <c r="D89" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E89" t="n">
-        <v>1.45</v>
+        <v>0.5</v>
       </c>
       <c r="F89" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G89" t="n">
-        <v>0.222</v>
+        <v>0.135</v>
+      </c>
+      <c r="I89" t="n">
+        <v>611</v>
       </c>
     </row>
     <row r="90">
@@ -2472,19 +2741,22 @@
         <v>20</v>
       </c>
       <c r="C90" t="n">
-        <v>349</v>
+        <v>373</v>
       </c>
       <c r="D90" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E90" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F90" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G90" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.131</v>
+      </c>
+      <c r="I90" t="n">
+        <v>613</v>
       </c>
     </row>
     <row r="91">
@@ -2495,19 +2767,22 @@
         <v>20</v>
       </c>
       <c r="C91" t="n">
-        <v>395</v>
+        <v>311</v>
       </c>
       <c r="D91" t="n">
+        <v>7</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F91" t="n">
         <v>9</v>
       </c>
-      <c r="E91" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="F91" t="n">
-        <v>10</v>
-      </c>
       <c r="G91" t="n">
-        <v>0.091</v>
+        <v>0.104</v>
+      </c>
+      <c r="I91" t="n">
+        <v>625</v>
       </c>
     </row>
     <row r="92">
@@ -2518,19 +2793,22 @@
         <v>20</v>
       </c>
       <c r="C92" t="n">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="D92" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E92" t="n">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="F92" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G92" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.108</v>
+      </c>
+      <c r="I92" t="n">
+        <v>631</v>
       </c>
     </row>
     <row r="93">
@@ -2541,19 +2819,22 @@
         <v>20</v>
       </c>
       <c r="C93" t="n">
-        <v>325</v>
+        <v>348</v>
       </c>
       <c r="D93" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E93" t="n">
-        <v>0.45</v>
+        <v>0.15</v>
       </c>
       <c r="F93" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G93" t="n">
-        <v>0.077</v>
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="I93" t="n">
+        <v>654</v>
       </c>
     </row>
     <row r="94">
@@ -2564,19 +2845,22 @@
         <v>20</v>
       </c>
       <c r="C94" t="n">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="D94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E94" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="F94" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G94" t="n">
-        <v>0.076</v>
+        <v>0.109</v>
+      </c>
+      <c r="I94" t="n">
+        <v>681</v>
       </c>
     </row>
     <row r="95">
@@ -2587,19 +2871,22 @@
         <v>20</v>
       </c>
       <c r="C95" t="n">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="D95" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E95" t="n">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="F95" t="n">
         <v>8</v>
       </c>
       <c r="G95" t="n">
-        <v>0.097</v>
+        <v>0.093</v>
+      </c>
+      <c r="I95" t="n">
+        <v>691</v>
       </c>
     </row>
     <row r="96">
@@ -2610,19 +2897,22 @@
         <v>20</v>
       </c>
       <c r="C96" t="n">
-        <v>351</v>
+        <v>307</v>
       </c>
       <c r="D96" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E96" t="n">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="F96" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G96" t="n">
-        <v>0.078</v>
+        <v>0.101</v>
+      </c>
+      <c r="I96" t="n">
+        <v>692</v>
       </c>
     </row>
     <row r="97">
@@ -2633,19 +2923,22 @@
         <v>20</v>
       </c>
       <c r="C97" t="n">
-        <v>363</v>
+        <v>303</v>
       </c>
       <c r="D97" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E97" t="n">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="F97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G97" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.163</v>
+      </c>
+      <c r="I97" t="n">
+        <v>697</v>
       </c>
     </row>
     <row r="98">
@@ -2656,19 +2949,22 @@
         <v>20</v>
       </c>
       <c r="C98" t="n">
-        <v>305</v>
+        <v>330</v>
       </c>
       <c r="D98" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E98" t="n">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="F98" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G98" t="n">
-        <v>0.066</v>
+        <v>0.08</v>
+      </c>
+      <c r="I98" t="n">
+        <v>702</v>
       </c>
     </row>
     <row r="99">
@@ -2679,19 +2975,22 @@
         <v>20</v>
       </c>
       <c r="C99" t="n">
-        <v>383</v>
+        <v>340</v>
       </c>
       <c r="D99" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E99" t="n">
-        <v>0.05</v>
+        <v>0.35</v>
       </c>
       <c r="F99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G99" t="n">
-        <v>0.048</v>
+        <v>0.082</v>
+      </c>
+      <c r="I99" t="n">
+        <v>711</v>
       </c>
     </row>
     <row r="100">
@@ -2702,7 +3001,7 @@
         <v>20</v>
       </c>
       <c r="C100" t="n">
-        <v>320</v>
+        <v>338</v>
       </c>
       <c r="D100" t="n">
         <v>2</v>
@@ -2711,10 +3010,13 @@
         <v>0.1</v>
       </c>
       <c r="F100" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G100" t="n">
-        <v>30.062</v>
+        <v>0.067</v>
+      </c>
+      <c r="I100" t="n">
+        <v>714</v>
       </c>
     </row>
     <row r="101">
@@ -2725,19 +3027,22 @@
         <v>20</v>
       </c>
       <c r="C101" t="n">
-        <v>363</v>
+        <v>281</v>
       </c>
       <c r="D101" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E101" t="n">
-        <v>0.65</v>
+        <v>0.05</v>
       </c>
       <c r="F101" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G101" t="n">
-        <v>30.113</v>
+        <v>0.07199999999999999</v>
+      </c>
+      <c r="I101" t="n">
+        <v>715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final push of the day
</commit_message>
<xml_diff>
--- a/distributed.xlsx
+++ b/distributed.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9169fa5a3c35e09c/Bureaublad/Jilles/AE/MSc/AE4422-20_Agent-based_modelling/ABMS_assignment_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_AED0D96E37FE773ADFFF799E0532D94B5752AD37" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D729D7C1-9383-478C-9921-52B8A14732A1}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_C3D4CCAD7061BD04B9BF689E0532D94B5752E0B4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34B4227A-C54F-4F54-A537-63F905FEE622}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="2085" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="2085" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Normal capacity" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Normal capacity" sheetId="1" r:id="rId1"/>
+    <sheet name="30-30 capacity" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Simulation run</t>
   </si>
@@ -35,6 +36,9 @@
     <t>Total waiting time [s]</t>
   </si>
   <si>
+    <t>Maximum delay</t>
+  </si>
+  <si>
     <t>Average waiting time [s]</t>
   </si>
   <si>
@@ -45,9 +49,6 @@
   </si>
   <si>
     <t>Seed</t>
-  </si>
-  <si>
-    <t>Maximum delay</t>
   </si>
 </sst>
 </file>
@@ -364,11 +365,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,19 +396,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3316,7 +3317,2951 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B02536-0421-436D-ADCA-097AFE828B22}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>414</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>0.2</v>
+      </c>
+      <c r="G2">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>562</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="I3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>533</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G4">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="I4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>510</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0.4</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="I5">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>445</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>0.11</v>
+      </c>
+      <c r="I6">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>511</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>0.3</v>
+      </c>
+      <c r="G7">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>0.153</v>
+      </c>
+      <c r="I7">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>530</v>
+      </c>
+      <c r="D8">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="G8">
+        <v>16</v>
+      </c>
+      <c r="H8">
+        <v>0.22</v>
+      </c>
+      <c r="I8">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>522</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="I9">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>493</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0.2</v>
+      </c>
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>0.153</v>
+      </c>
+      <c r="I10">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>512</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="G11">
+        <v>16</v>
+      </c>
+      <c r="H11">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="I11">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>482</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="I12">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>515</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>0.5</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="I13">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>475</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>0.11</v>
+      </c>
+      <c r="I14">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>512</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G15">
+        <v>12</v>
+      </c>
+      <c r="H15">
+        <v>0.156</v>
+      </c>
+      <c r="I15">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>513</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G16">
+        <v>18</v>
+      </c>
+      <c r="H16">
+        <v>0.17</v>
+      </c>
+      <c r="I16">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>514</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0.2</v>
+      </c>
+      <c r="G17">
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="I17">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>544</v>
+      </c>
+      <c r="D18">
+        <v>23</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="G18">
+        <v>12</v>
+      </c>
+      <c r="H18">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="I18">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>498</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G19">
+        <v>13</v>
+      </c>
+      <c r="H19">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="I19">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>529</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>0.5</v>
+      </c>
+      <c r="G20">
+        <v>14</v>
+      </c>
+      <c r="H20">
+        <v>0.251</v>
+      </c>
+      <c r="I20">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>30</v>
+      </c>
+      <c r="C21">
+        <v>468</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G21">
+        <v>13</v>
+      </c>
+      <c r="H21">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="I21">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <v>462</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G22">
+        <v>13</v>
+      </c>
+      <c r="H22">
+        <v>0.1</v>
+      </c>
+      <c r="I22">
+        <v>2297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <v>537</v>
+      </c>
+      <c r="D23">
+        <v>24</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>0.8</v>
+      </c>
+      <c r="G23">
+        <v>12</v>
+      </c>
+      <c r="H23">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="I23">
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>541</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>0.4</v>
+      </c>
+      <c r="G24">
+        <v>11</v>
+      </c>
+      <c r="H24">
+        <v>0.151</v>
+      </c>
+      <c r="I24">
+        <v>2403</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>565</v>
+      </c>
+      <c r="D25">
+        <v>13</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>0.433</v>
+      </c>
+      <c r="G25">
+        <v>14</v>
+      </c>
+      <c r="H25">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="I25">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <v>541</v>
+      </c>
+      <c r="D26">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>9</v>
+      </c>
+      <c r="F26">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="G26">
+        <v>13</v>
+      </c>
+      <c r="H26">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="I26">
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>30</v>
+      </c>
+      <c r="C27">
+        <v>551</v>
+      </c>
+      <c r="D27">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G27">
+        <v>16</v>
+      </c>
+      <c r="H27">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="I27">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>492</v>
+      </c>
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>0.4</v>
+      </c>
+      <c r="G28">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <v>0.156</v>
+      </c>
+      <c r="I28">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>513</v>
+      </c>
+      <c r="D29">
+        <v>18</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>0.6</v>
+      </c>
+      <c r="G29">
+        <v>13</v>
+      </c>
+      <c r="H29">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="I29">
+        <v>2494</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>30</v>
+      </c>
+      <c r="C30">
+        <v>520</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G30">
+        <v>12</v>
+      </c>
+      <c r="H30">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="I30">
+        <v>2839</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>516</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0.2</v>
+      </c>
+      <c r="G31">
+        <v>12</v>
+      </c>
+      <c r="H31">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="I31">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>558</v>
+      </c>
+      <c r="D32">
+        <v>19</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="G32">
+        <v>14</v>
+      </c>
+      <c r="H32">
+        <v>0.192</v>
+      </c>
+      <c r="I32">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>521</v>
+      </c>
+      <c r="D33">
+        <v>13</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>0.433</v>
+      </c>
+      <c r="G33">
+        <v>12</v>
+      </c>
+      <c r="H33">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="I33">
+        <v>3122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>484</v>
+      </c>
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G34">
+        <v>11</v>
+      </c>
+      <c r="H34">
+        <v>0.2</v>
+      </c>
+      <c r="I34">
+        <v>3133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>549</v>
+      </c>
+      <c r="D35">
+        <v>16</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="G35">
+        <v>15</v>
+      </c>
+      <c r="H35">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="I35">
+        <v>3287</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>30</v>
+      </c>
+      <c r="C36">
+        <v>493</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G36">
+        <v>10</v>
+      </c>
+      <c r="H36">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="I36">
+        <v>3298</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>30</v>
+      </c>
+      <c r="C37">
+        <v>515</v>
+      </c>
+      <c r="D37">
+        <v>12</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>0.4</v>
+      </c>
+      <c r="G37">
+        <v>16</v>
+      </c>
+      <c r="H37">
+        <v>0.15</v>
+      </c>
+      <c r="I37">
+        <v>3315</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>30</v>
+      </c>
+      <c r="C38">
+        <v>511</v>
+      </c>
+      <c r="D38">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0.3</v>
+      </c>
+      <c r="G38">
+        <v>16</v>
+      </c>
+      <c r="H38">
+        <v>0.161</v>
+      </c>
+      <c r="I38">
+        <v>3419</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>30</v>
+      </c>
+      <c r="C39">
+        <v>529</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G39">
+        <v>12</v>
+      </c>
+      <c r="H39">
+        <v>0.124</v>
+      </c>
+      <c r="I39">
+        <v>3435</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>30</v>
+      </c>
+      <c r="C40">
+        <v>491</v>
+      </c>
+      <c r="D40">
+        <v>9</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <v>0.3</v>
+      </c>
+      <c r="G40">
+        <v>11</v>
+      </c>
+      <c r="H40">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="I40">
+        <v>3516</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>30</v>
+      </c>
+      <c r="C41">
+        <v>561</v>
+      </c>
+      <c r="D41">
+        <v>12</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <v>0.4</v>
+      </c>
+      <c r="G41">
+        <v>12</v>
+      </c>
+      <c r="H41">
+        <v>0.19</v>
+      </c>
+      <c r="I41">
+        <v>3607</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>30</v>
+      </c>
+      <c r="C42">
+        <v>484</v>
+      </c>
+      <c r="D42">
+        <v>9</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>0.3</v>
+      </c>
+      <c r="G42">
+        <v>13</v>
+      </c>
+      <c r="H42">
+        <v>0.114</v>
+      </c>
+      <c r="I42">
+        <v>3668</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>30</v>
+      </c>
+      <c r="C43">
+        <v>583</v>
+      </c>
+      <c r="D43">
+        <v>14</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="G43">
+        <v>13</v>
+      </c>
+      <c r="H43">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="I43">
+        <v>3719</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>30</v>
+      </c>
+      <c r="C44">
+        <v>523</v>
+      </c>
+      <c r="D44">
+        <v>7</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G44">
+        <v>12</v>
+      </c>
+      <c r="H44">
+        <v>0.215</v>
+      </c>
+      <c r="I44">
+        <v>3868</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>30</v>
+      </c>
+      <c r="C45">
+        <v>487</v>
+      </c>
+      <c r="D45">
+        <v>7</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G45">
+        <v>14</v>
+      </c>
+      <c r="H45">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I45">
+        <v>3930</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>30</v>
+      </c>
+      <c r="C46">
+        <v>525</v>
+      </c>
+      <c r="D46">
+        <v>10</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G46">
+        <v>11</v>
+      </c>
+      <c r="H46">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="I46">
+        <v>3943</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>30</v>
+      </c>
+      <c r="C47">
+        <v>502</v>
+      </c>
+      <c r="D47">
+        <v>17</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="G47">
+        <v>12</v>
+      </c>
+      <c r="H47">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="I47">
+        <v>4042</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>30</v>
+      </c>
+      <c r="C48">
+        <v>514</v>
+      </c>
+      <c r="D48">
+        <v>7</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G48">
+        <v>13</v>
+      </c>
+      <c r="H48">
+        <v>0.157</v>
+      </c>
+      <c r="I48">
+        <v>4065</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>30</v>
+      </c>
+      <c r="C49">
+        <v>575</v>
+      </c>
+      <c r="D49">
+        <v>11</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G49">
+        <v>15</v>
+      </c>
+      <c r="H49">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="I49">
+        <v>4175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>30</v>
+      </c>
+      <c r="C50">
+        <v>509</v>
+      </c>
+      <c r="D50">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G50">
+        <v>10</v>
+      </c>
+      <c r="H50">
+        <v>0.106</v>
+      </c>
+      <c r="I50">
+        <v>4336</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>30</v>
+      </c>
+      <c r="C51">
+        <v>526</v>
+      </c>
+      <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G51">
+        <v>13</v>
+      </c>
+      <c r="H51">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I51">
+        <v>4381</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>30</v>
+      </c>
+      <c r="C52">
+        <v>503</v>
+      </c>
+      <c r="D52">
+        <v>12</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="F52">
+        <v>0.4</v>
+      </c>
+      <c r="G52">
+        <v>12</v>
+      </c>
+      <c r="H52">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="I52">
+        <v>4412</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>30</v>
+      </c>
+      <c r="C53">
+        <v>576</v>
+      </c>
+      <c r="D53">
+        <v>14</v>
+      </c>
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="G53">
+        <v>17</v>
+      </c>
+      <c r="H53">
+        <v>0.153</v>
+      </c>
+      <c r="I53">
+        <v>4525</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>30</v>
+      </c>
+      <c r="C54">
+        <v>503</v>
+      </c>
+      <c r="D54">
+        <v>12</v>
+      </c>
+      <c r="E54">
+        <v>5</v>
+      </c>
+      <c r="F54">
+        <v>0.4</v>
+      </c>
+      <c r="G54">
+        <v>10</v>
+      </c>
+      <c r="H54">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="I54">
+        <v>4536</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>30</v>
+      </c>
+      <c r="C55">
+        <v>517</v>
+      </c>
+      <c r="D55">
+        <v>8</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G55">
+        <v>12</v>
+      </c>
+      <c r="H55">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="I55">
+        <v>4635</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>30</v>
+      </c>
+      <c r="C56">
+        <v>491</v>
+      </c>
+      <c r="D56">
+        <v>11</v>
+      </c>
+      <c r="E56">
+        <v>4</v>
+      </c>
+      <c r="F56">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G56">
+        <v>11</v>
+      </c>
+      <c r="H56">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="I56">
+        <v>4715</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>30</v>
+      </c>
+      <c r="C57">
+        <v>495</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G57">
+        <v>10</v>
+      </c>
+      <c r="H57">
+        <v>0.113</v>
+      </c>
+      <c r="I57">
+        <v>4862</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>30</v>
+      </c>
+      <c r="C58">
+        <v>530</v>
+      </c>
+      <c r="D58">
+        <v>11</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G58">
+        <v>14</v>
+      </c>
+      <c r="H58">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="I58">
+        <v>5020</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>30</v>
+      </c>
+      <c r="C59">
+        <v>490</v>
+      </c>
+      <c r="D59">
+        <v>6</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>0.2</v>
+      </c>
+      <c r="G59">
+        <v>13</v>
+      </c>
+      <c r="H59">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="I59">
+        <v>5082</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>30</v>
+      </c>
+      <c r="C60">
+        <v>483</v>
+      </c>
+      <c r="D60">
+        <v>4</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G60">
+        <v>13</v>
+      </c>
+      <c r="H60">
+        <v>0.121</v>
+      </c>
+      <c r="I60">
+        <v>5115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>30</v>
+      </c>
+      <c r="C61">
+        <v>512</v>
+      </c>
+      <c r="D61">
+        <v>11</v>
+      </c>
+      <c r="E61">
+        <v>6</v>
+      </c>
+      <c r="F61">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G61">
+        <v>11</v>
+      </c>
+      <c r="H61">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I61">
+        <v>5128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>30</v>
+      </c>
+      <c r="C62">
+        <v>531</v>
+      </c>
+      <c r="D62">
+        <v>9</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62">
+        <v>0.3</v>
+      </c>
+      <c r="G62">
+        <v>13</v>
+      </c>
+      <c r="H62">
+        <v>0.15</v>
+      </c>
+      <c r="I62">
+        <v>5182</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>30</v>
+      </c>
+      <c r="C63">
+        <v>526</v>
+      </c>
+      <c r="D63">
+        <v>10</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G63">
+        <v>12</v>
+      </c>
+      <c r="H63">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="I63">
+        <v>5361</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>30</v>
+      </c>
+      <c r="C64">
+        <v>492</v>
+      </c>
+      <c r="D64">
+        <v>9</v>
+      </c>
+      <c r="E64">
+        <v>4</v>
+      </c>
+      <c r="F64">
+        <v>0.3</v>
+      </c>
+      <c r="G64">
+        <v>13</v>
+      </c>
+      <c r="H64">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I64">
+        <v>5585</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>30</v>
+      </c>
+      <c r="C65">
+        <v>542</v>
+      </c>
+      <c r="D65">
+        <v>11</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="F65">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G65">
+        <v>13</v>
+      </c>
+      <c r="H65">
+        <v>0.152</v>
+      </c>
+      <c r="I65">
+        <v>5655</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>30</v>
+      </c>
+      <c r="C66">
+        <v>511</v>
+      </c>
+      <c r="D66">
+        <v>12</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="F66">
+        <v>0.4</v>
+      </c>
+      <c r="G66">
+        <v>12</v>
+      </c>
+      <c r="H66">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="I66">
+        <v>5723</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>30</v>
+      </c>
+      <c r="C67">
+        <v>487</v>
+      </c>
+      <c r="D67">
+        <v>14</v>
+      </c>
+      <c r="E67">
+        <v>5</v>
+      </c>
+      <c r="F67">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="G67">
+        <v>13</v>
+      </c>
+      <c r="H67">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="I67">
+        <v>5782</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>30</v>
+      </c>
+      <c r="C68">
+        <v>498</v>
+      </c>
+      <c r="D68">
+        <v>12</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68">
+        <v>0.4</v>
+      </c>
+      <c r="G68">
+        <v>11</v>
+      </c>
+      <c r="H68">
+        <v>0.214</v>
+      </c>
+      <c r="I68">
+        <v>5830</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>30</v>
+      </c>
+      <c r="C69">
+        <v>533</v>
+      </c>
+      <c r="D69">
+        <v>8</v>
+      </c>
+      <c r="E69">
+        <v>4</v>
+      </c>
+      <c r="F69">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G69">
+        <v>14</v>
+      </c>
+      <c r="H69">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="I69">
+        <v>5873</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>30</v>
+      </c>
+      <c r="C70">
+        <v>501</v>
+      </c>
+      <c r="D70">
+        <v>6</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70">
+        <v>0.2</v>
+      </c>
+      <c r="G70">
+        <v>12</v>
+      </c>
+      <c r="H70">
+        <v>0.127</v>
+      </c>
+      <c r="I70">
+        <v>5892</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>30</v>
+      </c>
+      <c r="C71">
+        <v>542</v>
+      </c>
+      <c r="D71">
+        <v>6</v>
+      </c>
+      <c r="E71">
+        <v>3</v>
+      </c>
+      <c r="F71">
+        <v>0.2</v>
+      </c>
+      <c r="G71">
+        <v>12</v>
+      </c>
+      <c r="H71">
+        <v>0.253</v>
+      </c>
+      <c r="I71">
+        <v>5936</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>30</v>
+      </c>
+      <c r="C72">
+        <v>538</v>
+      </c>
+      <c r="D72">
+        <v>11</v>
+      </c>
+      <c r="E72">
+        <v>4</v>
+      </c>
+      <c r="F72">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G72">
+        <v>12</v>
+      </c>
+      <c r="H72">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="I72">
+        <v>6339</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>30</v>
+      </c>
+      <c r="C73">
+        <v>531</v>
+      </c>
+      <c r="D73">
+        <v>14</v>
+      </c>
+      <c r="E73">
+        <v>5</v>
+      </c>
+      <c r="F73">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="G73">
+        <v>12</v>
+      </c>
+      <c r="H73">
+        <v>0.15</v>
+      </c>
+      <c r="I73">
+        <v>6368</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>30</v>
+      </c>
+      <c r="C74">
+        <v>508</v>
+      </c>
+      <c r="D74">
+        <v>7</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="F74">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G74">
+        <v>12</v>
+      </c>
+      <c r="H74">
+        <v>0.438</v>
+      </c>
+      <c r="I74">
+        <v>6369</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>30</v>
+      </c>
+      <c r="C75">
+        <v>543</v>
+      </c>
+      <c r="D75">
+        <v>7</v>
+      </c>
+      <c r="E75">
+        <v>3</v>
+      </c>
+      <c r="F75">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G75">
+        <v>15</v>
+      </c>
+      <c r="H75">
+        <v>0.18</v>
+      </c>
+      <c r="I75">
+        <v>6496</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>30</v>
+      </c>
+      <c r="C76">
+        <v>539</v>
+      </c>
+      <c r="D76">
+        <v>12</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="F76">
+        <v>0.4</v>
+      </c>
+      <c r="G76">
+        <v>13</v>
+      </c>
+      <c r="H76">
+        <v>0.41</v>
+      </c>
+      <c r="I76">
+        <v>6503</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>30</v>
+      </c>
+      <c r="C77">
+        <v>562</v>
+      </c>
+      <c r="D77">
+        <v>13</v>
+      </c>
+      <c r="E77">
+        <v>4</v>
+      </c>
+      <c r="F77">
+        <v>0.433</v>
+      </c>
+      <c r="G77">
+        <v>13</v>
+      </c>
+      <c r="H77">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="I77">
+        <v>6583</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>30</v>
+      </c>
+      <c r="C78">
+        <v>516</v>
+      </c>
+      <c r="D78">
+        <v>14</v>
+      </c>
+      <c r="E78">
+        <v>3</v>
+      </c>
+      <c r="F78">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="G78">
+        <v>15</v>
+      </c>
+      <c r="H78">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="I78">
+        <v>6621</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>30</v>
+      </c>
+      <c r="C79">
+        <v>518</v>
+      </c>
+      <c r="D79">
+        <v>7</v>
+      </c>
+      <c r="E79">
+        <v>3</v>
+      </c>
+      <c r="F79">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G79">
+        <v>11</v>
+      </c>
+      <c r="H79">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="I79">
+        <v>6652</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>30</v>
+      </c>
+      <c r="C80">
+        <v>493</v>
+      </c>
+      <c r="D80">
+        <v>11</v>
+      </c>
+      <c r="E80">
+        <v>3</v>
+      </c>
+      <c r="F80">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G80">
+        <v>13</v>
+      </c>
+      <c r="H80">
+        <v>0.115</v>
+      </c>
+      <c r="I80">
+        <v>6681</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>30</v>
+      </c>
+      <c r="C81">
+        <v>566</v>
+      </c>
+      <c r="D81">
+        <v>11</v>
+      </c>
+      <c r="E81">
+        <v>5</v>
+      </c>
+      <c r="F81">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G81">
+        <v>16</v>
+      </c>
+      <c r="H81">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I81">
+        <v>6713</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>30</v>
+      </c>
+      <c r="C82">
+        <v>529</v>
+      </c>
+      <c r="D82">
+        <v>8</v>
+      </c>
+      <c r="E82">
+        <v>3</v>
+      </c>
+      <c r="F82">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G82">
+        <v>14</v>
+      </c>
+      <c r="H82">
+        <v>0.15</v>
+      </c>
+      <c r="I82">
+        <v>6770</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>30</v>
+      </c>
+      <c r="C83">
+        <v>478</v>
+      </c>
+      <c r="D83">
+        <v>7</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="F83">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G83">
+        <v>13</v>
+      </c>
+      <c r="H83">
+        <v>0.17</v>
+      </c>
+      <c r="I83">
+        <v>6787</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>30</v>
+      </c>
+      <c r="C84">
+        <v>477</v>
+      </c>
+      <c r="D84">
+        <v>8</v>
+      </c>
+      <c r="E84">
+        <v>3</v>
+      </c>
+      <c r="F84">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G84">
+        <v>11</v>
+      </c>
+      <c r="H84">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="I84">
+        <v>6790</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>30</v>
+      </c>
+      <c r="C85">
+        <v>551</v>
+      </c>
+      <c r="D85">
+        <v>20</v>
+      </c>
+      <c r="E85">
+        <v>6</v>
+      </c>
+      <c r="F85">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="G85">
+        <v>14</v>
+      </c>
+      <c r="H85">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="I85">
+        <v>6850</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>30</v>
+      </c>
+      <c r="C86">
+        <v>520</v>
+      </c>
+      <c r="D86">
+        <v>5</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G86">
+        <v>14</v>
+      </c>
+      <c r="H86">
+        <v>0.128</v>
+      </c>
+      <c r="I86">
+        <v>6866</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>30</v>
+      </c>
+      <c r="C87">
+        <v>484</v>
+      </c>
+      <c r="D87">
+        <v>8</v>
+      </c>
+      <c r="E87">
+        <v>3</v>
+      </c>
+      <c r="F87">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G87">
+        <v>10</v>
+      </c>
+      <c r="H87">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="I87">
+        <v>6943</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>30</v>
+      </c>
+      <c r="C88">
+        <v>517</v>
+      </c>
+      <c r="D88">
+        <v>6</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="F88">
+        <v>0.2</v>
+      </c>
+      <c r="G88">
+        <v>14</v>
+      </c>
+      <c r="H88">
+        <v>0.161</v>
+      </c>
+      <c r="I88">
+        <v>6999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>30</v>
+      </c>
+      <c r="C89">
+        <v>522</v>
+      </c>
+      <c r="D89">
+        <v>17</v>
+      </c>
+      <c r="E89">
+        <v>4</v>
+      </c>
+      <c r="F89">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="G89">
+        <v>12</v>
+      </c>
+      <c r="H89">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="I89">
+        <v>7185</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>30</v>
+      </c>
+      <c r="C90">
+        <v>542</v>
+      </c>
+      <c r="D90">
+        <v>15</v>
+      </c>
+      <c r="E90">
+        <v>5</v>
+      </c>
+      <c r="F90">
+        <v>0.5</v>
+      </c>
+      <c r="G90">
+        <v>13</v>
+      </c>
+      <c r="H90">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="I90">
+        <v>7439</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>30</v>
+      </c>
+      <c r="C91">
+        <v>517</v>
+      </c>
+      <c r="D91">
+        <v>12</v>
+      </c>
+      <c r="E91">
+        <v>4</v>
+      </c>
+      <c r="F91">
+        <v>0.4</v>
+      </c>
+      <c r="G91">
+        <v>15</v>
+      </c>
+      <c r="H91">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I91">
+        <v>7561</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>30</v>
+      </c>
+      <c r="C92">
+        <v>579</v>
+      </c>
+      <c r="D92">
+        <v>13</v>
+      </c>
+      <c r="E92">
+        <v>3</v>
+      </c>
+      <c r="F92">
+        <v>0.433</v>
+      </c>
+      <c r="G92">
+        <v>14</v>
+      </c>
+      <c r="H92">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="I92">
+        <v>7612</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>30</v>
+      </c>
+      <c r="C93">
+        <v>512</v>
+      </c>
+      <c r="D93">
+        <v>4</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G93">
+        <v>11</v>
+      </c>
+      <c r="H93">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="I93">
+        <v>7618</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>30</v>
+      </c>
+      <c r="C94">
+        <v>489</v>
+      </c>
+      <c r="D94">
+        <v>7</v>
+      </c>
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G94">
+        <v>12</v>
+      </c>
+      <c r="H94">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="I94">
+        <v>7622</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>30</v>
+      </c>
+      <c r="C95">
+        <v>505</v>
+      </c>
+      <c r="D95">
+        <v>6</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>0.2</v>
+      </c>
+      <c r="G95">
+        <v>12</v>
+      </c>
+      <c r="H95">
+        <v>0.112</v>
+      </c>
+      <c r="I95">
+        <v>7639</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>30</v>
+      </c>
+      <c r="C96">
+        <v>548</v>
+      </c>
+      <c r="D96">
+        <v>15</v>
+      </c>
+      <c r="E96">
+        <v>3</v>
+      </c>
+      <c r="F96">
+        <v>0.5</v>
+      </c>
+      <c r="G96">
+        <v>13</v>
+      </c>
+      <c r="H96">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="I96">
+        <v>7682</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>30</v>
+      </c>
+      <c r="C97">
+        <v>514</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G97">
+        <v>12</v>
+      </c>
+      <c r="H97">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="I97">
+        <v>7691</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>30</v>
+      </c>
+      <c r="C98">
+        <v>505</v>
+      </c>
+      <c r="D98">
+        <v>11</v>
+      </c>
+      <c r="E98">
+        <v>5</v>
+      </c>
+      <c r="F98">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G98">
+        <v>12</v>
+      </c>
+      <c r="H98">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="I98">
+        <v>7831</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>30</v>
+      </c>
+      <c r="C99">
+        <v>457</v>
+      </c>
+      <c r="D99">
+        <v>3</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>0.1</v>
+      </c>
+      <c r="G99">
+        <v>10</v>
+      </c>
+      <c r="H99">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="I99">
+        <v>8051</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>30</v>
+      </c>
+      <c r="C100">
+        <v>544</v>
+      </c>
+      <c r="D100">
+        <v>24</v>
+      </c>
+      <c r="E100">
+        <v>8</v>
+      </c>
+      <c r="F100">
+        <v>0.8</v>
+      </c>
+      <c r="G100">
+        <v>12</v>
+      </c>
+      <c r="H100">
+        <v>0.252</v>
+      </c>
+      <c r="I100">
+        <v>8092</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>30</v>
+      </c>
+      <c r="C101">
+        <v>507</v>
+      </c>
+      <c r="D101">
+        <v>8</v>
+      </c>
+      <c r="E101">
+        <v>2</v>
+      </c>
+      <c r="F101">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G101">
+        <v>16</v>
+      </c>
+      <c r="H101">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="I101">
+        <v>8162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74AB7FB-8EC4-41A7-A8C3-7541244F6A38}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
cleaned up code, updated distributed.xlsx
</commit_message>
<xml_diff>
--- a/distributed.xlsx
+++ b/distributed.xlsx
@@ -8,21 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9169fa5a3c35e09c/Bureaublad/Jilles/AE/MSc/AE4422-20_Agent-based_modelling/ABMS_assignment_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_C3D4CCAD7061BD04B9BF689E0532D94B5752E0B4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34B4227A-C54F-4F54-A537-63F905FEE622}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_C3D4CCAD7061BD04B9BF689E0532D94B5752E0B4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F00AE652-B099-4E81-AB89-5D27C84BB887}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="2085" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3480" yWindow="2910" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Normal capacity" sheetId="1" r:id="rId1"/>
     <sheet name="30-30 capacity" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Simulation run</t>
   </si>
@@ -50,13 +61,33 @@
   <si>
     <t>Seed</t>
   </si>
+  <si>
+    <t>High demand</t>
+  </si>
+  <si>
+    <t>Low demand</t>
+  </si>
+  <si>
+    <t>High demand (Approx)</t>
+  </si>
+  <si>
+    <t>Numb. Of Aircraft</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,8 +115,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,9 +412,16 @@
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,7 +450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -440,7 +479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -469,7 +508,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -498,7 +537,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -526,8 +565,31 @@
       <c r="I5">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" t="str">
+        <f>C1</f>
+        <v>Total cost</v>
+      </c>
+      <c r="N5" t="str">
+        <f>D1</f>
+        <v>Total waiting time [s]</v>
+      </c>
+      <c r="O5" t="str">
+        <f>E1</f>
+        <v>Maximum delay</v>
+      </c>
+      <c r="P5" t="str">
+        <f>F1</f>
+        <v>Average waiting time [s]</v>
+      </c>
+      <c r="Q5" t="str">
+        <f>G1</f>
+        <v>Maximum capacity</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -555,8 +617,34 @@
       <c r="I6">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="1">
+        <v>40</v>
+      </c>
+      <c r="M6" s="1">
+        <f>M7+M7-M8</f>
+        <v>488.83</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" ref="N6:Q6" si="0">N7+N7-N8</f>
+        <v>8.41</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="0"/>
+        <v>6.2</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2205</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="0"/>
+        <v>12.77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -584,8 +672,34 @@
       <c r="I7">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <f>'30-30 capacity'!C2</f>
+        <v>414</v>
+      </c>
+      <c r="N7">
+        <f>'30-30 capacity'!D2</f>
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <f>'30-30 capacity'!E2</f>
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <f>'30-30 capacity'!F2</f>
+        <v>0.2</v>
+      </c>
+      <c r="Q7">
+        <f>'30-30 capacity'!G2</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -613,8 +727,34 @@
       <c r="I8">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>20</v>
+      </c>
+      <c r="M8">
+        <f>AVERAGE(C:C)</f>
+        <v>339.17</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ref="N8:Q8" si="1">AVERAGE(D:D)</f>
+        <v>3.59</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>0.17950000000000002</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>9.23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -643,7 +783,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -672,7 +812,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -701,7 +841,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -730,7 +870,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -759,7 +899,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -788,7 +928,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -817,7 +957,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6264,7 +6404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74AB7FB-8EC4-41A7-A8C3-7541244F6A38}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>